<commit_message>
Updating 1988.xlsx with updated flag paths
</commit_message>
<xml_diff>
--- a/resources/1988.xlsx
+++ b/resources/1988.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aditya/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aditya/Development/melbourne-qt/melbourne/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E7FAA8-6147-8247-B500-435DBBD56F92}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE4F2D1-A1DC-A24B-8EEA-B027EC9F1D23}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1820" windowWidth="25740" windowHeight="14300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -237,67 +237,67 @@
     <t>Mangup</t>
   </si>
   <si>
-    <t>Square/is.png</t>
-  </si>
-  <si>
-    <t>Square/se.png</t>
-  </si>
-  <si>
-    <t>Square/fi.png</t>
-  </si>
-  <si>
-    <t>Square/gb.png</t>
-  </si>
-  <si>
-    <t>Square/tr.png</t>
-  </si>
-  <si>
-    <t>Square/es.png</t>
-  </si>
-  <si>
-    <t>Square/nl.png</t>
-  </si>
-  <si>
-    <t>Square/il.png</t>
-  </si>
-  <si>
-    <t>Square/ch.png</t>
-  </si>
-  <si>
-    <t>Square/ie.png</t>
-  </si>
-  <si>
-    <t>Square/de.png</t>
-  </si>
-  <si>
-    <t>Square/at.png</t>
-  </si>
-  <si>
-    <t>Square/dk.png</t>
-  </si>
-  <si>
-    <t>Square/gr.png</t>
-  </si>
-  <si>
-    <t>Square/no.png</t>
-  </si>
-  <si>
-    <t>Square/be.png</t>
-  </si>
-  <si>
-    <t>Square/lu.png</t>
-  </si>
-  <si>
-    <t>Square/it.png</t>
-  </si>
-  <si>
-    <t>Square/fr.png</t>
-  </si>
-  <si>
-    <t>Square/pt.png</t>
-  </si>
-  <si>
-    <t>Square/rs.png</t>
+    <t>World/is.png</t>
+  </si>
+  <si>
+    <t>World/se.png</t>
+  </si>
+  <si>
+    <t>World/fi.png</t>
+  </si>
+  <si>
+    <t>World/gb.png</t>
+  </si>
+  <si>
+    <t>World/tr.png</t>
+  </si>
+  <si>
+    <t>World/es.png</t>
+  </si>
+  <si>
+    <t>World/nl.png</t>
+  </si>
+  <si>
+    <t>World/il.png</t>
+  </si>
+  <si>
+    <t>World/ch.png</t>
+  </si>
+  <si>
+    <t>World/ie.png</t>
+  </si>
+  <si>
+    <t>World/de.png</t>
+  </si>
+  <si>
+    <t>World/at.png</t>
+  </si>
+  <si>
+    <t>World/dk.png</t>
+  </si>
+  <si>
+    <t>World/gr.png</t>
+  </si>
+  <si>
+    <t>World/no.png</t>
+  </si>
+  <si>
+    <t>World/be.png</t>
+  </si>
+  <si>
+    <t>World/lu.png</t>
+  </si>
+  <si>
+    <t>World/it.png</t>
+  </si>
+  <si>
+    <t>World/fr.png</t>
+  </si>
+  <si>
+    <t>World/pt.png</t>
+  </si>
+  <si>
+    <t>World/rs.png</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
   <dimension ref="A1:AA22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>